<commit_message>
Added report and sketches
Report is done, need more sketches
</commit_message>
<xml_diff>
--- a/Data summary.xlsx
+++ b/Data summary.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/nguc_ucalgary_ca/Documents/CPSC 583/A3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chi_n\Documents\GitHub\583_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="6B49373956D6C446F61A1873AE9461E7DE3E1210" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{A0984B26-A3BB-4BDE-B0C5-DE14D54CD6D7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="102">
   <si>
     <t>State</t>
   </si>
@@ -329,18 +328,6 @@
   </si>
   <si>
     <t>weight</t>
-  </si>
-  <si>
-    <t>% from</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t>cereal obesity poverty</t>
@@ -703,7 +690,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
@@ -730,9 +717,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
@@ -2129,10 +2113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:D32"/>
+      <selection activeCell="A7" sqref="A7:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,12 +2135,12 @@
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>82</v>
       </c>
@@ -2214,11 +2198,8 @@
       <c r="S2" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="X2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
@@ -2276,19 +2257,8 @@
       <c r="S3" s="13">
         <v>1</v>
       </c>
-      <c r="V3" t="s">
-        <v>102</v>
-      </c>
-      <c r="W3">
-        <f>4*H7</f>
-        <v>88</v>
-      </c>
-      <c r="X3">
-        <f>W3/120</f>
-        <v>0.73333333333333328</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>70</v>
       </c>
@@ -2346,19 +2316,8 @@
       <c r="S4" s="15">
         <v>30</v>
       </c>
-      <c r="V4" t="s">
-        <v>103</v>
-      </c>
-      <c r="W4">
-        <f>9*J7</f>
-        <v>27</v>
-      </c>
-      <c r="X4">
-        <f t="shared" ref="X4:X5" si="0">W4/120</f>
-        <v>0.22500000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>66</v>
       </c>
@@ -2416,19 +2375,8 @@
       <c r="S5" s="15">
         <v>1</v>
       </c>
-      <c r="V5" t="s">
-        <v>104</v>
-      </c>
-      <c r="W5">
-        <f>4</f>
-        <v>4</v>
-      </c>
-      <c r="X5">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>68</v>
       </c>
@@ -2486,511 +2434,507 @@
       <c r="S6" s="15">
         <v>1</v>
       </c>
-      <c r="W6">
-        <f>SUM(W3:W5)</f>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7">
         <v>22.5</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7">
         <v>120</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7">
         <v>22</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7">
         <v>0.8</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7">
         <v>70</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7">
         <v>42</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7">
         <v>3</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7">
         <v>90</v>
       </c>
-      <c r="Q7" s="27">
+      <c r="Q7">
         <v>9</v>
       </c>
-      <c r="R7" s="27">
+      <c r="R7">
         <v>15</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B10" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B14" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>105</v>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>58</v>
+      <c r="A18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="10">
+        <v>78.7</v>
+      </c>
+      <c r="C18" s="10">
+        <v>44.7</v>
+      </c>
+      <c r="D18" s="10">
+        <v>22.2</v>
+      </c>
+      <c r="E18" s="10">
+        <v>33.1</v>
+      </c>
+      <c r="F18" s="15">
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="10">
-        <v>78.7</v>
+        <v>69.7</v>
       </c>
       <c r="C19" s="10">
-        <v>44.7</v>
+        <v>30.9</v>
       </c>
       <c r="D19" s="10">
-        <v>22.2</v>
+        <v>28.7</v>
       </c>
       <c r="E19" s="10">
-        <v>33.1</v>
+        <v>40.4</v>
       </c>
       <c r="F19" s="15">
-        <v>18.100000000000001</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="10">
-        <v>69.7</v>
+        <v>83.3</v>
       </c>
       <c r="C20" s="10">
-        <v>30.9</v>
+        <v>38</v>
       </c>
       <c r="D20" s="10">
-        <v>28.7</v>
+        <v>26</v>
       </c>
       <c r="E20" s="10">
-        <v>40.4</v>
+        <v>36</v>
       </c>
       <c r="F20" s="15">
-        <v>17.3</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" s="10">
-        <v>83.3</v>
+        <v>68.2</v>
       </c>
       <c r="C21" s="10">
+        <v>31.9</v>
+      </c>
+      <c r="D21" s="10">
+        <v>32.6</v>
+      </c>
+      <c r="E21" s="10">
+        <v>35.5</v>
+      </c>
+      <c r="F21" s="15">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="17">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="C22" s="17">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="D22" s="17">
+        <v>25.1</v>
+      </c>
+      <c r="E22" s="17">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="F22" s="18">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="10">
-        <v>26</v>
-      </c>
-      <c r="E21" s="10">
-        <v>36</v>
-      </c>
-      <c r="F21" s="15">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="10">
-        <v>68.2</v>
-      </c>
-      <c r="C22" s="10">
-        <v>31.9</v>
-      </c>
-      <c r="D22" s="10">
-        <v>32.6</v>
-      </c>
-      <c r="E22" s="10">
-        <v>35.5</v>
-      </c>
-      <c r="F22" s="15">
-        <v>21.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="17">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="C23" s="17">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="D23" s="17">
-        <v>25.1</v>
-      </c>
-      <c r="E23" s="17">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="F23" s="18">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>61</v>
-      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="L26" s="20"/>
-      <c r="M26" s="21"/>
+      <c r="A26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>78</v>
+        <v>4</v>
+      </c>
+      <c r="B27" s="10">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C27" s="10">
+        <v>28.4</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>80</v>
+        <v>24</v>
+      </c>
+      <c r="E27" s="10">
+        <v>41.6</v>
+      </c>
+      <c r="F27" s="10">
+        <v>12.7</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="H27" s="10">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="I27" s="10">
+        <v>26.4</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="K27" s="10">
+        <v>35</v>
+      </c>
+      <c r="L27" s="10">
+        <v>12.5</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28" s="10">
-        <v>18.600000000000001</v>
+        <v>29.6</v>
       </c>
       <c r="C28" s="10">
-        <v>28.4</v>
+        <v>31.1</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E28" s="10">
-        <v>41.6</v>
+        <v>36.6</v>
       </c>
       <c r="F28" s="10">
-        <v>12.7</v>
+        <v>23.4</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H28" s="10">
-        <v>17.600000000000001</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="I28" s="10">
-        <v>26.4</v>
+        <v>32.9</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K28" s="10">
-        <v>35</v>
+        <v>37.1</v>
       </c>
       <c r="L28" s="10">
-        <v>12.5</v>
+        <v>35.4</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" s="10">
-        <v>29.6</v>
+        <v>28.4</v>
       </c>
       <c r="C29" s="10">
+        <v>22.9</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="10">
+        <v>23.3</v>
+      </c>
+      <c r="F29" s="10">
+        <v>22</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="10">
+        <v>27.8</v>
+      </c>
+      <c r="I29" s="10">
+        <v>24.3</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="10">
         <v>31.1</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="10">
-        <v>36.6</v>
-      </c>
-      <c r="F29" s="10">
-        <v>23.4</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="10">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="I29" s="10">
-        <v>32.9</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K29" s="10">
-        <v>37.1</v>
-      </c>
       <c r="L29" s="10">
-        <v>35.4</v>
+        <v>23.2</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B30" s="10">
-        <v>28.4</v>
+        <v>32.4</v>
       </c>
       <c r="C30" s="10">
-        <v>22.9</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E30" s="10">
-        <v>23.3</v>
+        <v>37.6</v>
       </c>
       <c r="F30" s="10">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H30" s="10">
-        <v>27.8</v>
+        <v>33.5</v>
       </c>
       <c r="I30" s="10">
-        <v>24.3</v>
+        <v>31.2</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K30" s="10">
-        <v>31.1</v>
+        <v>43.1</v>
       </c>
       <c r="L30" s="10">
-        <v>23.2</v>
+        <v>30.5</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" s="10">
-        <v>32.4</v>
+        <v>28.3</v>
       </c>
       <c r="C31" s="10">
-        <v>37.299999999999997</v>
+        <v>24.1</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E31" s="10">
-        <v>37.6</v>
+        <v>30.9</v>
       </c>
       <c r="F31" s="10">
-        <v>29</v>
+        <v>24.3</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H31" s="10">
-        <v>33.5</v>
+        <v>28</v>
       </c>
       <c r="I31" s="10">
-        <v>31.2</v>
+        <v>24.6</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K31" s="10">
-        <v>43.1</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="L31" s="10">
-        <v>30.5</v>
+        <v>22.8</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="10">
-        <v>28.3</v>
-      </c>
-      <c r="C32" s="10">
-        <v>24.1</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="10">
-        <v>30.9</v>
-      </c>
-      <c r="F32" s="10">
-        <v>24.3</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H32" s="10">
-        <v>28</v>
-      </c>
-      <c r="I32" s="10">
-        <v>24.6</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K32" s="10">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="L32" s="10">
-        <v>22.8</v>
-      </c>
-      <c r="M32" s="10" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>